<commit_message>
finish inital calculations and documentation
</commit_message>
<xml_diff>
--- a/calculations/environments/environments.xlsx
+++ b/calculations/environments/environments.xlsx
@@ -8,13 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sucha\programming\offset_me\calculations\environments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59089A1D-9242-4C69-AE05-C512CAEA4BB6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6ED88B5-B814-4BC9-B453-70D348694B95}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16845" yWindow="6000" windowWidth="21600" windowHeight="11385" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Forrest_loss" sheetId="1" r:id="rId1"/>
     <sheet name="climate" sheetId="2" r:id="rId2"/>
+    <sheet name="biodiversity" sheetId="3" r:id="rId3"/>
+    <sheet name="nitrogen_phosphorus_cycles" sheetId="4" r:id="rId4"/>
+    <sheet name="freshwater" sheetId="5" r:id="rId5"/>
+    <sheet name="chemical_pollution" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -57,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="91">
   <si>
     <t>per UK person</t>
   </si>
@@ -207,6 +211,129 @@
   </si>
   <si>
     <t>taking £10k per km2 lost</t>
+  </si>
+  <si>
+    <t>global shortfall (USD)</t>
+  </si>
+  <si>
+    <t>per uk person (GBP)</t>
+  </si>
+  <si>
+    <t>Fertilizer market size</t>
+  </si>
+  <si>
+    <t>average profit margins</t>
+  </si>
+  <si>
+    <t>runoff-rate</t>
+  </si>
+  <si>
+    <t>cost to reduce</t>
+  </si>
+  <si>
+    <t>per capita in gbp</t>
+  </si>
+  <si>
+    <t>Arable land for livestock feed</t>
+  </si>
+  <si>
+    <t>runoff fertilizer reduction from switching to vegan</t>
+  </si>
+  <si>
+    <t>Meat consumption rate UK vs global</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Mid</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>agriculture water use rate</t>
+  </si>
+  <si>
+    <t>of which for livestock feed</t>
+  </si>
+  <si>
+    <t>reduction by going vegan</t>
+  </si>
+  <si>
+    <t>Plastics</t>
+  </si>
+  <si>
+    <t>Going to landfills</t>
+  </si>
+  <si>
+    <t>Going to mismanaged coastal</t>
+  </si>
+  <si>
+    <t>Going into the ocean</t>
+  </si>
+  <si>
+    <t>Incineration</t>
+  </si>
+  <si>
+    <t>OceanCleanup</t>
+  </si>
+  <si>
+    <t>$/kg</t>
+  </si>
+  <si>
+    <t>overall cost</t>
+  </si>
+  <si>
+    <t>equal proportion</t>
+  </si>
+  <si>
+    <t>proportion by income</t>
+  </si>
+  <si>
+    <t>proportion by uk consumption</t>
+  </si>
+  <si>
+    <t>tCO2/kg</t>
+  </si>
+  <si>
+    <t>15$/tCO2</t>
+  </si>
+  <si>
+    <t>cost per kg</t>
+  </si>
+  <si>
+    <t>capital cost per tonne of annual capacity</t>
+  </si>
+  <si>
+    <t>world</t>
+  </si>
+  <si>
+    <t>UK per capita</t>
+  </si>
+  <si>
+    <t>Recycling projects</t>
+  </si>
+  <si>
+    <t>Annual waste production</t>
+  </si>
+  <si>
+    <t>med</t>
+  </si>
+  <si>
+    <t>POPs</t>
+  </si>
+  <si>
+    <t>Others</t>
+  </si>
+  <si>
+    <t>DDT phase out cost to developing nations</t>
+  </si>
+  <si>
+    <t>low est</t>
+  </si>
+  <si>
+    <t>high est</t>
   </si>
 </sst>
 </file>
@@ -242,10 +369,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,8 +656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1360,10 +1488,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70C63200-0F8F-430F-8C89-AEE905A7D7DD}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1423,6 +1551,9 @@
       <c r="C6" t="s">
         <v>48</v>
       </c>
+      <c r="D6" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" cm="1">
@@ -1434,8 +1565,8 @@
         <v>151.23780945236308</v>
       </c>
       <c r="D7">
-        <f>B2*15*0.74</f>
-        <v>133.23330832708177</v>
+        <f>B2*F8</f>
+        <v>133.23330832708174</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1456,6 +1587,620 @@
       </c>
       <c r="C9">
         <v>217.46974350291185</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <f>B8</f>
+        <v>31.714285714285715</v>
+      </c>
+      <c r="C12">
+        <f>D7</f>
+        <v>133.23330832708174</v>
+      </c>
+      <c r="D12">
+        <f>C9</f>
+        <v>217.46974350291185</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96AFF124-469E-48B4-8235-5F906E866836}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2">
+        <v>3400000000</v>
+      </c>
+      <c r="C2">
+        <v>12700000000</v>
+      </c>
+      <c r="D2" s="3">
+        <v>38100000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3">
+        <f>B2*Forrest_loss!$B5*0.74</f>
+        <v>1.3159063844476337</v>
+      </c>
+      <c r="C3">
+        <f>C2*Forrest_loss!$B5*0.74</f>
+        <v>4.9152973772014557</v>
+      </c>
+      <c r="D3">
+        <f>D2*Forrest_loss!$B5*0.74</f>
+        <v>14.745892131604368</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D143D82-4FEE-4819-824A-7303C1AEF487}">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>158000000000</v>
+      </c>
+      <c r="B2">
+        <v>0.3</v>
+      </c>
+      <c r="C2">
+        <v>0.5</v>
+      </c>
+      <c r="D2">
+        <f>C2*A2*B2</f>
+        <v>23700000000</v>
+      </c>
+      <c r="E2">
+        <f>D2*Forrest_loss!B5*0.74</f>
+        <v>9.1726415621790949</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0.36</v>
+      </c>
+      <c r="B5">
+        <v>0.7</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <f>1/(A5*B5*C5/7600000000)</f>
+        <v>15079365079.36508</v>
+      </c>
+      <c r="E5">
+        <f>D5*Forrest_loss!B5*0.74</f>
+        <v>5.836186112162709</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f>B8/2</f>
+        <v>2.9180930560813545</v>
+      </c>
+      <c r="B8">
+        <f>E5</f>
+        <v>5.836186112162709</v>
+      </c>
+      <c r="C8">
+        <f>E2*2</f>
+        <v>18.34528312435819</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C5F5C85-0EAB-461B-A55F-BB6029F37BA9}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="10.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0.92</v>
+      </c>
+      <c r="B2">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="C2">
+        <v>0.8</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <f>1/(A2*C2*B2*D2/7600000000)</f>
+        <v>17803598200.899551</v>
+      </c>
+      <c r="F2">
+        <f>E2*Forrest_loss!B5*0.74</f>
+        <v>6.8905495702070976</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <f>C7/2</f>
+        <v>1.7226373925517744</v>
+      </c>
+      <c r="C7">
+        <f>D7/2</f>
+        <v>3.4452747851035488</v>
+      </c>
+      <c r="D7">
+        <f>F2</f>
+        <v>6.8905495702070976</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D7AE5D9-62B8-4D5D-8A52-33A5526DF1A0}">
+  <dimension ref="A1:J27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27:H27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3">
+        <v>415000000000</v>
+      </c>
+      <c r="D3">
+        <f>0.21*365</f>
+        <v>76.649999999999991</v>
+      </c>
+      <c r="E3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H3" t="s">
+        <v>71</v>
+      </c>
+      <c r="I3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4">
+        <v>201000000000</v>
+      </c>
+      <c r="E4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F4">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="G4" t="s">
+        <v>72</v>
+      </c>
+      <c r="H4">
+        <v>5</v>
+      </c>
+      <c r="I4">
+        <f>I5/C4</f>
+        <v>3.283582089552239</v>
+      </c>
+      <c r="J4">
+        <f>J5/C4</f>
+        <v>0.46766169154228854</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5">
+        <v>37600000000</v>
+      </c>
+      <c r="D5">
+        <f>C5*(0.0021/3+0.0014*2/3)/68000000</f>
+        <v>0.90313725490196084</v>
+      </c>
+      <c r="E5" t="s">
+        <v>80</v>
+      </c>
+      <c r="F5">
+        <v>1000</v>
+      </c>
+      <c r="G5" t="s">
+        <v>73</v>
+      </c>
+      <c r="H5">
+        <f>C6*H4</f>
+        <v>47000000000</v>
+      </c>
+      <c r="I5">
+        <v>660000000000</v>
+      </c>
+      <c r="J5">
+        <v>94000000000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6">
+        <v>9400000000</v>
+      </c>
+      <c r="E6" t="s">
+        <v>79</v>
+      </c>
+      <c r="F6">
+        <f>F4*climate!F8+F5/20/1000</f>
+        <v>7.775E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F8">
+        <f>0.74*F6/7600000000*C4</f>
+        <v>1.5216493421052633</v>
+      </c>
+      <c r="H8">
+        <f>0.74*H5/7600000000</f>
+        <v>4.5763157894736839</v>
+      </c>
+      <c r="I8">
+        <f t="shared" ref="I8:J8" si="0">0.74*I5/7600000000</f>
+        <v>64.263157894736835</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>9.1526315789473678</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9">
+        <f>0.74*F6*Forrest_loss!B5*C4</f>
+        <v>6.0484282351622092</v>
+      </c>
+      <c r="H9">
+        <f>0.74*H5*Forrest_loss!$B5</f>
+        <v>18.190470608540821</v>
+      </c>
+      <c r="I9">
+        <f>0.74*I5*Forrest_loss!$B5</f>
+        <v>255.44065109865835</v>
+      </c>
+      <c r="J9">
+        <f>0.74*J5*Forrest_loss!$B5</f>
+        <v>36.380941217081642</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10">
+        <v>0.02</v>
+      </c>
+      <c r="F10">
+        <f>(($D$5*7600000000/$C$5+$C10)*$D$3)*F$6</f>
+        <v>1.2070984779411764</v>
+      </c>
+      <c r="H10">
+        <f>($C10*($C$5/$C$3*$D$3)+$D$5)*H$4*0.74</f>
+        <v>3.855513770848098</v>
+      </c>
+      <c r="I10">
+        <f>($C10*($C$4/$C$3*$D$3)+$D$5*$C$4/$C$5)*I$4*0.74</f>
+        <v>13.535314301913539</v>
+      </c>
+      <c r="J10">
+        <f>($C10*($C$4/$C$3*$D$3)+$D$5*$C$4/$C$5)*J$4*0.74</f>
+        <v>1.9277568854240494</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>0.1</v>
+      </c>
+      <c r="F11">
+        <f t="shared" ref="F11:F12" si="1">(($D$5*7600000000/$C$5+$C11)*$D$3)*F$6</f>
+        <v>1.6838614779411765</v>
+      </c>
+      <c r="H11">
+        <f t="shared" ref="H11:H12" si="2">($C11*($C$5/$C$3*$D$3)+$D$5)*H$4*0.74</f>
+        <v>5.9111374816914717</v>
+      </c>
+      <c r="I11">
+        <f>($C11*($C$4/$C$3*$D$3)+$D$5*$C$4/$C$5)*I$4*0.74</f>
+        <v>20.751865627214741</v>
+      </c>
+      <c r="J11">
+        <f>($C11*($C$4/$C$3*$D$3)+$D$5*$C$4/$C$5)*J$4*0.74</f>
+        <v>2.9555687408457358</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>0.2</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>2.2798152279411763</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="2"/>
+        <v>8.4806671202456876</v>
+      </c>
+      <c r="I12">
+        <f>($C12*($C$4/$C$3*$D$3)+$D$5*$C$4/$C$5)*I$4*0.74</f>
+        <v>29.772554783841251</v>
+      </c>
+      <c r="J12">
+        <f>($C12*($C$4/$C$3*$D$3)+$D$5*$C$4/$C$5)*J$4*0.74</f>
+        <v>4.2403335601228447</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" t="s">
+        <v>85</v>
+      </c>
+      <c r="H14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <f>AVERAGE(H10,J10)</f>
+        <v>2.8916353281360738</v>
+      </c>
+      <c r="G15">
+        <f>AVERAGE(H12,J12)</f>
+        <v>6.3605003401842666</v>
+      </c>
+      <c r="H15">
+        <f>AVERAGE(H9,J9)</f>
+        <v>27.285705912811231</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>89</v>
+      </c>
+      <c r="C19" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="3">
+        <v>350000000</v>
+      </c>
+      <c r="C20" s="3">
+        <v>950000000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>32</v>
+      </c>
+      <c r="G22" t="s">
+        <v>85</v>
+      </c>
+      <c r="H22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F23" s="3">
+        <f>B20*Forrest_loss!$B5*0.74</f>
+        <v>0.13546095134019762</v>
+      </c>
+      <c r="G23" s="3">
+        <f>C20*Forrest_loss!$B5*0.74</f>
+        <v>0.36767972506625063</v>
+      </c>
+      <c r="H23" s="3">
+        <f>C20*Forrest_loss!$B5*0.74*2</f>
+        <v>0.73535945013250126</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F26" t="s">
+        <v>32</v>
+      </c>
+      <c r="G26" t="s">
+        <v>85</v>
+      </c>
+      <c r="H26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F27">
+        <f>1000000000*Forrest_loss!B5*0.74</f>
+        <v>0.3870312895434217</v>
+      </c>
+      <c r="G27">
+        <f>10000000000*Forrest_loss!B5*0.74</f>
+        <v>3.8703128954342172</v>
+      </c>
+      <c r="H27">
+        <f>50000000000*Forrest_loss!B5*0.74</f>
+        <v>19.351564477171088</v>
       </c>
     </row>
   </sheetData>

</xml_diff>